<commit_message>
Updated notes on trapping rain solution,
</commit_message>
<xml_diff>
--- a/LeetCode/Documents/trappingRain.xlsx
+++ b/LeetCode/Documents/trappingRain.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomb\source\repos\cs.leetcode\LeetCode\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BA55D44-E37C-46A5-B5B6-6FC6272994D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED29898C-79E6-4233-91B9-946CB8A08630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="4740" windowWidth="28800" windowHeight="15435" xr2:uid="{B6B83340-0371-42C9-8F2C-2FD214984665}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B6B83340-0371-42C9-8F2C-2FD214984665}"/>
   </bookViews>
   <sheets>
     <sheet name="TrappingRain" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Test 1</t>
   </si>
@@ -47,6 +47,129 @@
   </si>
   <si>
     <t>Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ok so the idea here was to break this array up into substrings. If I can get the two highest points in the array, I can calculate the water held there, then discard that part of the array. </t>
+  </si>
+  <si>
+    <t>So I start by finding the highest point, at index x, then find the highest point in the subarray to the left, so [ : x]. Say that's index y. Now we know that x is high and y is high, we can calculate the water between these indices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then we can discard the array [y:x], and continue working with [ :y], and [x: ]. </t>
+  </si>
+  <si>
+    <t>How does that look for our example.</t>
+  </si>
+  <si>
+    <t>leftStart</t>
+  </si>
+  <si>
+    <t>leftEnd</t>
+  </si>
+  <si>
+    <t>leftMax</t>
+  </si>
+  <si>
+    <t>leftMaxIndex</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>maxIndex</t>
+  </si>
+  <si>
+    <t>rightStart</t>
+  </si>
+  <si>
+    <t>rightEnd</t>
+  </si>
+  <si>
+    <t>rightMax</t>
+  </si>
+  <si>
+    <t>rightMaxIndex</t>
+  </si>
+  <si>
+    <t>We use these to track the sub arrays we're working with.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1 find a max, this is 3 at index 7. It doesn't matter if this max is duplicated through the array. We just want to find one potential wall. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We've set leftEnd to (maxIndex - 1) and leftStart to 0. </t>
+  </si>
+  <si>
+    <t>We iterate i down from leftEnd until it = leftStart (0), and grab the max value.</t>
+  </si>
+  <si>
+    <t>We can see that this would be 2 at index 3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then we set leftStart to leftMaxIndex (3), to work out the area held by the walls at 3 and 7. </t>
+  </si>
+  <si>
+    <t>We sum the values of the array from leftStart to leftEnd, in this case (2, 1, 0, 1).</t>
+  </si>
+  <si>
+    <t>The get the area of a rectangle height leftMax, and length (leftEnd-leftStart) + 1.</t>
+  </si>
+  <si>
+    <t>We can then subtract the sum of heights, from this rectangle to get the blue area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is added to the rainfall total. </t>
+  </si>
+  <si>
+    <t>Ok next!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then work through the sub array to the left of max. So at this point we have a wall at 7, if we find a wall in our new sub array, we know that it's a left wall. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We need to move left to handle the rest of the array on this side. </t>
+  </si>
+  <si>
+    <t>leftEnd = leftMaxIndex - 1</t>
+  </si>
+  <si>
+    <t>leftStart = 0 again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same deal here, if we find the max in this subarray we know it's a left wall, given the previous leftMaxIndex (3), is to the right of this index. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">So we iterate through the array from leftEnd down to leftStart, and find leftMaxIndex = 1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum the values of the array from [1:2], get the total area of the rectangle (2), take the values away to get 1, add it to rainfall. </t>
+  </si>
+  <si>
+    <t>Then we set leftEnd to leftMaxIndex - 1, which is 0. And we only loop while leftEnd &gt; 1.</t>
+  </si>
+  <si>
+    <t>If leftEnd = 1, or less, there's not enough indices left to catch water.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So we're done with the left side. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To look at the right we do the same thing working up from the max. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find the max in the sub array [8:11], it's at 8 and 10. Now because of the way the loop that checks this works, it sets rightMax at the furthest right of the maximum values. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this case that's 10. </t>
+  </si>
+  <si>
+    <t>Same with the left side, sum the values, take em from the area of the rectangle.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Then we set rightStart to rightMaxIndex + 1, which is beyond our while test of &gt; length - 1, so we're done. </t>
+  </si>
+  <si>
+    <t>I set up a bunch of variables here to make it easier to track. I actually reckon I can simplify this significantly. So we have</t>
   </si>
 </sst>
 </file>
@@ -62,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,8 +204,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -119,11 +266,79 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -133,6 +348,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E977B707-0AEE-43C9-8D64-A8377CC06B0F}">
-  <dimension ref="A2:M7"/>
+  <dimension ref="A2:M109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,6 +801,959 @@
       </c>
       <c r="M7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>3</v>
+      </c>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>2</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="E33" s="12"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>0</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>6</v>
+      </c>
+      <c r="I35">
+        <v>7</v>
+      </c>
+      <c r="J35">
+        <v>8</v>
+      </c>
+      <c r="K35">
+        <v>9</v>
+      </c>
+      <c r="L35">
+        <v>10</v>
+      </c>
+      <c r="M35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <v>2</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>3</v>
+      </c>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>0</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>6</v>
+      </c>
+      <c r="I48">
+        <v>7</v>
+      </c>
+      <c r="J48">
+        <v>8</v>
+      </c>
+      <c r="K48">
+        <v>9</v>
+      </c>
+      <c r="L48">
+        <v>10</v>
+      </c>
+      <c r="M48">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>2</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>3</v>
+      </c>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>2</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>1</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="L64" s="9"/>
+    </row>
+    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>0</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66">
+        <v>4</v>
+      </c>
+      <c r="G66">
+        <v>5</v>
+      </c>
+      <c r="H66">
+        <v>6</v>
+      </c>
+      <c r="I66">
+        <v>7</v>
+      </c>
+      <c r="J66">
+        <v>8</v>
+      </c>
+      <c r="K66">
+        <v>9</v>
+      </c>
+      <c r="L66">
+        <v>10</v>
+      </c>
+      <c r="M66">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <v>1</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>3</v>
+      </c>
+      <c r="J67">
+        <v>2</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>2</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>3</v>
+      </c>
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>2</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>1</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="L75" s="9"/>
+    </row>
+    <row r="76" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>0</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77">
+        <v>3</v>
+      </c>
+      <c r="F77">
+        <v>4</v>
+      </c>
+      <c r="G77">
+        <v>5</v>
+      </c>
+      <c r="H77">
+        <v>6</v>
+      </c>
+      <c r="I77">
+        <v>7</v>
+      </c>
+      <c r="J77">
+        <v>8</v>
+      </c>
+      <c r="K77">
+        <v>9</v>
+      </c>
+      <c r="L77">
+        <v>10</v>
+      </c>
+      <c r="M77">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>3</v>
+      </c>
+      <c r="J78">
+        <v>2</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
+      </c>
+      <c r="L78">
+        <v>2</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>3</v>
+      </c>
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>2</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="I90" s="9"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>1</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="25"/>
+      <c r="H91" s="25"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="12"/>
+      <c r="L91" s="12"/>
+    </row>
+    <row r="92" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>0</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="11"/>
+      <c r="K92" s="11"/>
+      <c r="L92" s="11"/>
+      <c r="M92" s="11"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="F93">
+        <v>4</v>
+      </c>
+      <c r="G93">
+        <v>5</v>
+      </c>
+      <c r="H93">
+        <v>6</v>
+      </c>
+      <c r="I93">
+        <v>7</v>
+      </c>
+      <c r="J93">
+        <v>8</v>
+      </c>
+      <c r="K93">
+        <v>9</v>
+      </c>
+      <c r="L93">
+        <v>10</v>
+      </c>
+      <c r="M93">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>3</v>
+      </c>
+      <c r="J94">
+        <v>2</v>
+      </c>
+      <c r="K94">
+        <v>1</v>
+      </c>
+      <c r="L94">
+        <v>2</v>
+      </c>
+      <c r="M94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>14</v>
+      </c>
+      <c r="M95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>3</v>
+      </c>
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>2</v>
+      </c>
+      <c r="B101" s="3"/>
+      <c r="I101" s="9"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>1</v>
+      </c>
+      <c r="B102" s="3"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="25"/>
+      <c r="H102" s="25"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="13"/>
+      <c r="K102" s="23"/>
+      <c r="L102" s="22"/>
+    </row>
+    <row r="103" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>0</v>
+      </c>
+      <c r="B103" s="4"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="14"/>
+      <c r="K103" s="11"/>
+      <c r="L103" s="15"/>
+      <c r="M103" s="10"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+      <c r="E104">
+        <v>3</v>
+      </c>
+      <c r="F104">
+        <v>4</v>
+      </c>
+      <c r="G104">
+        <v>5</v>
+      </c>
+      <c r="H104">
+        <v>6</v>
+      </c>
+      <c r="I104">
+        <v>7</v>
+      </c>
+      <c r="J104">
+        <v>8</v>
+      </c>
+      <c r="K104">
+        <v>9</v>
+      </c>
+      <c r="L104">
+        <v>10</v>
+      </c>
+      <c r="M104">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+      <c r="I105">
+        <v>3</v>
+      </c>
+      <c r="J105">
+        <v>2</v>
+      </c>
+      <c r="K105">
+        <v>1</v>
+      </c>
+      <c r="L105">
+        <v>2</v>
+      </c>
+      <c r="M105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>14</v>
+      </c>
+      <c r="L106" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated left/rightmaxIndex initialisation to actually mean something now lol.
</commit_message>
<xml_diff>
--- a/LeetCode/Documents/trappingRain.xlsx
+++ b/LeetCode/Documents/trappingRain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomb\source\repos\cs.leetcode\LeetCode\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED29898C-79E6-4233-91B9-946CB8A08630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BF6FD4-9603-43CC-A4F0-0C504E620CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B6B83340-0371-42C9-8F2C-2FD214984665}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Test 1</t>
   </si>
@@ -100,9 +100,6 @@
     <t xml:space="preserve">We've set leftEnd to (maxIndex - 1) and leftStart to 0. </t>
   </si>
   <si>
-    <t>We iterate i down from leftEnd until it = leftStart (0), and grab the max value.</t>
-  </si>
-  <si>
     <t>We can see that this would be 2 at index 3.</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t xml:space="preserve">To look at the right we do the same thing working up from the max. </t>
   </si>
   <si>
-    <t xml:space="preserve">Find the max in the sub array [8:11], it's at 8 and 10. Now because of the way the loop that checks this works, it sets rightMax at the furthest right of the maximum values. </t>
-  </si>
-  <si>
     <t xml:space="preserve">In this case that's 10. </t>
   </si>
   <si>
@@ -170,6 +164,18 @@
   </si>
   <si>
     <t>I set up a bunch of variables here to make it easier to track. I actually reckon I can simplify this significantly. So we have</t>
+  </si>
+  <si>
+    <t>Find the max in the sub array [8:11], it's at 8 and 10.</t>
+  </si>
+  <si>
+    <t>We iterate i down from leftEnd until it = leftStart (0), and grab the max value. Now because of the way the loop that checks this works, it sets leftMax at the furthest left of the maximum values. If there are multiple identical maximums, this matters.</t>
+  </si>
+  <si>
+    <t>We've got a test after finding the max, if the leftMaxIndex isn't set to something less than leftEnd (ie an index in the current subarray), we can break. This would happen if everything in the subarray is zero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This obvs can't hold any water, so we move on. </t>
   </si>
 </sst>
 </file>
@@ -679,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E977B707-0AEE-43C9-8D64-A8377CC06B0F}">
-  <dimension ref="A2:M109"/>
+  <dimension ref="A2:M111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +831,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -878,7 +884,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,748 +1018,758 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>3</v>
-      </c>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>2</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="I45" s="9"/>
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B46" s="3"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
-        <v>0</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="I47" s="9"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>0</v>
-      </c>
-      <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-      <c r="E48">
-        <v>3</v>
-      </c>
-      <c r="F48">
+      <c r="A48" s="2">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>0</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50">
         <v>4</v>
       </c>
-      <c r="G48">
+      <c r="G50">
         <v>5</v>
       </c>
-      <c r="H48">
+      <c r="H50">
         <v>6</v>
       </c>
-      <c r="I48">
+      <c r="I50">
         <v>7</v>
       </c>
-      <c r="J48">
+      <c r="J50">
         <v>8</v>
       </c>
-      <c r="K48">
+      <c r="K50">
         <v>9</v>
       </c>
-      <c r="L48">
+      <c r="L50">
         <v>10</v>
       </c>
-      <c r="M48">
+      <c r="M50">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>0</v>
-      </c>
-      <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49">
-        <v>3</v>
-      </c>
-      <c r="J49">
-        <v>2</v>
-      </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49">
-        <v>2</v>
-      </c>
-      <c r="M49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
         <v>8</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H52" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>3</v>
-      </c>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>2</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="I63" s="9"/>
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B64" s="3"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="9"/>
-      <c r="J64" s="9"/>
-      <c r="L64" s="9"/>
-    </row>
-    <row r="65" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>0</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="10"/>
-      <c r="F65" s="10"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
-      <c r="L65" s="10"/>
-      <c r="M65" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="I65" s="9"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B66">
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-      <c r="D66">
-        <v>2</v>
-      </c>
-      <c r="E66">
-        <v>3</v>
-      </c>
-      <c r="F66">
+      <c r="A66" s="2">
+        <v>1</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="L66" s="9"/>
+    </row>
+    <row r="67" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>0</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
         <v>4</v>
       </c>
-      <c r="G66">
+      <c r="G68">
         <v>5</v>
       </c>
-      <c r="H66">
+      <c r="H68">
         <v>6</v>
       </c>
-      <c r="I66">
+      <c r="I68">
         <v>7</v>
       </c>
-      <c r="J66">
+      <c r="J68">
         <v>8</v>
       </c>
-      <c r="K66">
+      <c r="K68">
         <v>9</v>
       </c>
-      <c r="L66">
+      <c r="L68">
         <v>10</v>
       </c>
-      <c r="M66">
+      <c r="M68">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67">
-        <v>0</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-      <c r="E67">
-        <v>2</v>
-      </c>
-      <c r="F67">
-        <v>1</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>1</v>
-      </c>
-      <c r="I67">
-        <v>3</v>
-      </c>
-      <c r="J67">
-        <v>2</v>
-      </c>
-      <c r="K67">
-        <v>1</v>
-      </c>
-      <c r="L67">
-        <v>2</v>
-      </c>
-      <c r="M67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>2</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>3</v>
+      </c>
+      <c r="J69">
+        <v>2</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>2</v>
+      </c>
+      <c r="M69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>8</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D70" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <v>3</v>
-      </c>
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
-        <v>2</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B75" s="3"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="9"/>
-      <c r="J75" s="9"/>
-      <c r="L75" s="9"/>
-    </row>
-    <row r="76" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>0</v>
-      </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="10"/>
-      <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-      <c r="L76" s="10"/>
-      <c r="M76" s="10"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B77">
-        <v>0</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77">
-        <v>2</v>
-      </c>
-      <c r="E77">
-        <v>3</v>
-      </c>
-      <c r="F77">
+        <v>2</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>1</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="L77" s="9"/>
+    </row>
+    <row r="78" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>0</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+      <c r="F79">
         <v>4</v>
       </c>
-      <c r="G77">
+      <c r="G79">
         <v>5</v>
       </c>
-      <c r="H77">
+      <c r="H79">
         <v>6</v>
       </c>
-      <c r="I77">
+      <c r="I79">
         <v>7</v>
       </c>
-      <c r="J77">
+      <c r="J79">
         <v>8</v>
       </c>
-      <c r="K77">
+      <c r="K79">
         <v>9</v>
       </c>
-      <c r="L77">
+      <c r="L79">
         <v>10</v>
       </c>
-      <c r="M77">
+      <c r="M79">
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B78">
-        <v>0</v>
-      </c>
-      <c r="C78">
-        <v>1</v>
-      </c>
-      <c r="D78">
-        <v>0</v>
-      </c>
-      <c r="E78">
-        <v>2</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78">
-        <v>3</v>
-      </c>
-      <c r="J78">
-        <v>2</v>
-      </c>
-      <c r="K78">
-        <v>1</v>
-      </c>
-      <c r="L78">
-        <v>2</v>
-      </c>
-      <c r="M78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>3</v>
+      </c>
+      <c r="J80">
+        <v>2</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>2</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>8</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D81" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
-        <v>3</v>
-      </c>
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>2</v>
-      </c>
-      <c r="B90" s="3"/>
-      <c r="I90" s="9"/>
+      <c r="A89" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B91" s="3"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
-      <c r="I91" s="9"/>
-      <c r="J91" s="12"/>
-      <c r="L91" s="12"/>
-    </row>
-    <row r="92" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>0</v>
-      </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="10"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="10"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="10"/>
-      <c r="I92" s="10"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
-      <c r="L92" s="11"/>
-      <c r="M92" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="I92" s="9"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B93">
-        <v>0</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93">
-        <v>2</v>
-      </c>
-      <c r="E93">
-        <v>3</v>
-      </c>
-      <c r="F93">
+      <c r="A93" s="2">
+        <v>1</v>
+      </c>
+      <c r="B93" s="3"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="25"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="12"/>
+      <c r="L93" s="12"/>
+    </row>
+    <row r="94" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>0</v>
+      </c>
+      <c r="B94" s="4"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="11"/>
+      <c r="L94" s="11"/>
+      <c r="M94" s="11"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
+      <c r="E95">
+        <v>3</v>
+      </c>
+      <c r="F95">
         <v>4</v>
       </c>
-      <c r="G93">
+      <c r="G95">
         <v>5</v>
       </c>
-      <c r="H93">
+      <c r="H95">
         <v>6</v>
       </c>
-      <c r="I93">
+      <c r="I95">
         <v>7</v>
       </c>
-      <c r="J93">
+      <c r="J95">
         <v>8</v>
       </c>
-      <c r="K93">
+      <c r="K95">
         <v>9</v>
       </c>
-      <c r="L93">
+      <c r="L95">
         <v>10</v>
       </c>
-      <c r="M93">
+      <c r="M95">
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B94">
-        <v>0</v>
-      </c>
-      <c r="C94">
-        <v>1</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="E94">
-        <v>2</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>1</v>
-      </c>
-      <c r="I94">
-        <v>3</v>
-      </c>
-      <c r="J94">
-        <v>2</v>
-      </c>
-      <c r="K94">
-        <v>1</v>
-      </c>
-      <c r="L94">
-        <v>2</v>
-      </c>
-      <c r="M94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J95" t="s">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96">
+        <v>1</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96">
+        <v>3</v>
+      </c>
+      <c r="J96">
+        <v>2</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>2</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
         <v>14</v>
       </c>
-      <c r="M95" t="s">
+      <c r="M97" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>41</v>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
-        <v>3</v>
-      </c>
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2">
-        <v>2</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="I101" s="9"/>
+      <c r="A100" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B102" s="3"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="25"/>
-      <c r="G102" s="25"/>
-      <c r="H102" s="25"/>
-      <c r="I102" s="9"/>
-      <c r="J102" s="13"/>
-      <c r="K102" s="23"/>
-      <c r="L102" s="22"/>
     </row>
     <row r="103" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
-        <v>0</v>
-      </c>
-      <c r="B103" s="4"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="24"/>
-      <c r="E103" s="10"/>
-      <c r="F103" s="10"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="10"/>
-      <c r="I103" s="10"/>
-      <c r="J103" s="14"/>
-      <c r="K103" s="11"/>
-      <c r="L103" s="15"/>
-      <c r="M103" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="B103" s="3"/>
+      <c r="I103" s="9"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B104">
-        <v>0</v>
-      </c>
-      <c r="C104">
-        <v>1</v>
-      </c>
-      <c r="D104">
-        <v>2</v>
-      </c>
-      <c r="E104">
-        <v>3</v>
-      </c>
-      <c r="F104">
+      <c r="A104" s="2">
+        <v>1</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="13"/>
+      <c r="K104" s="23"/>
+      <c r="L104" s="22"/>
+    </row>
+    <row r="105" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>0</v>
+      </c>
+      <c r="B105" s="4"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="14"/>
+      <c r="K105" s="11"/>
+      <c r="L105" s="15"/>
+      <c r="M105" s="10"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>0</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <v>3</v>
+      </c>
+      <c r="F106">
         <v>4</v>
       </c>
-      <c r="G104">
+      <c r="G106">
         <v>5</v>
       </c>
-      <c r="H104">
+      <c r="H106">
         <v>6</v>
       </c>
-      <c r="I104">
+      <c r="I106">
         <v>7</v>
       </c>
-      <c r="J104">
+      <c r="J106">
         <v>8</v>
       </c>
-      <c r="K104">
+      <c r="K106">
         <v>9</v>
       </c>
-      <c r="L104">
+      <c r="L106">
         <v>10</v>
       </c>
-      <c r="M104">
+      <c r="M106">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B105">
-        <v>0</v>
-      </c>
-      <c r="C105">
-        <v>1</v>
-      </c>
-      <c r="D105">
-        <v>0</v>
-      </c>
-      <c r="E105">
-        <v>2</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105">
-        <v>1</v>
-      </c>
-      <c r="I105">
-        <v>3</v>
-      </c>
-      <c r="J105">
-        <v>2</v>
-      </c>
-      <c r="K105">
-        <v>1</v>
-      </c>
-      <c r="L105">
-        <v>2</v>
-      </c>
-      <c r="M105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J106" t="s">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>0</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>2</v>
+      </c>
+      <c r="F107">
+        <v>1</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>3</v>
+      </c>
+      <c r="J107">
+        <v>2</v>
+      </c>
+      <c r="K107">
+        <v>1</v>
+      </c>
+      <c r="L107">
+        <v>2</v>
+      </c>
+      <c r="M107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
         <v>14</v>
       </c>
-      <c r="L106" t="s">
+      <c r="L108" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>43</v>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>